<commit_message>
Fixed Jimmy's name because his last name is weird
</commit_message>
<xml_diff>
--- a/Data Sheet.xlsx
+++ b/Data Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="District" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -348,16 +348,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -676,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -913,10 +913,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="E2" s="1">
         <v>6000</v>
       </c>
@@ -940,7 +940,7 @@
       <c r="A4" s="2">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3"/>
@@ -949,7 +949,7 @@
       <c r="A5" s="2">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="3"/>
@@ -970,7 +970,7 @@
       <c r="A7" s="2">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3"/>
@@ -979,7 +979,7 @@
       <c r="A8" s="2">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3"/>
@@ -992,11 +992,11 @@
       <c r="C9" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" s="4">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="C2" s="1">
         <v>294</v>
@@ -1046,38 +1046,38 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <f>127006*C2*D2/1000000</f>
         <v>5600.9646000000002</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <f>730000*B2/1000000</f>
-        <v>4380</v>
-      </c>
-      <c r="C6" s="11" t="s">
+        <v>6570</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <f>B5-B6</f>
-        <v>1220.9646000000002</v>
-      </c>
-      <c r="C7" s="11" t="s">
+        <v>-969.03539999999975</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed useless time stuff and organized Data Sheet
</commit_message>
<xml_diff>
--- a/Data Sheet.xlsx
+++ b/Data Sheet.xlsx
@@ -12,8 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3590"/>
   </bookViews>
   <sheets>
-    <sheet name="District" sheetId="1" r:id="rId1"/>
-    <sheet name="Food" sheetId="5" r:id="rId2"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
+    <sheet name="Districts" sheetId="7" r:id="rId2"/>
+    <sheet name="Budget" sheetId="6" r:id="rId3"/>
+    <sheet name="Agriculture" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t xml:space="preserve">Tom </t>
   </si>
@@ -159,9 +161,6 @@
     <t>Total Calories Produced</t>
   </si>
   <si>
-    <t>Leftover Corn</t>
-  </si>
-  <si>
     <t>Total Calories Consumed</t>
   </si>
   <si>
@@ -214,6 +213,27 @@
   </si>
   <si>
     <t>F.D.</t>
+  </si>
+  <si>
+    <t>Time (year)</t>
+  </si>
+  <si>
+    <t>Time (minutes)</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>31.7515 kg of corn per bushel</t>
+  </si>
+  <si>
+    <t>4000 cal per kg</t>
+  </si>
+  <si>
+    <t>Leftover Corn (in kg)</t>
   </si>
 </sst>
 </file>
@@ -405,10 +425,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -727,367 +747,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.08984375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6328125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.90625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="B1" s="11" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <f>Districts!C2+Districts!C3+Districts!C4+Districts!C5+Districts!C6+Districts!C7+Districts!C8+Districts!C9</f>
+        <v>3318344</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="11">
+        <f>D2/30</f>
+        <v>8</v>
+      </c>
+      <c r="D2" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="12">
-        <f>C6+C7+C8+C9+C10+C11+C12+C13</f>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <v>6688494000</v>
+      </c>
+      <c r="B6" s="20">
+        <f>Budget!C1-Budget!G1</f>
         <v>3318344</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C6" s="11">
         <v>5</v>
       </c>
-      <c r="D2" s="12">
-        <v>6688494000</v>
-      </c>
-      <c r="E2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F2" s="21">
-        <f>C15-G15</f>
-        <v>3318344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5"/>
-      <c r="G5" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12">
-        <v>259000</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="12">
-        <v>571500</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="11">
-        <v>3</v>
-      </c>
-      <c r="C8" s="12">
-        <v>14344</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="11">
-        <v>4</v>
-      </c>
-      <c r="C9" s="12">
-        <v>571500</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="11">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12">
-        <v>571500</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="11">
-        <v>6</v>
-      </c>
-      <c r="C11" s="12">
-        <v>571500</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="11">
-        <v>7</v>
-      </c>
-      <c r="C12" s="12">
-        <v>259000</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="12">
-        <v>500000</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="20">
-        <f>C16+C17+C18+C19+C20+C21+C22</f>
-        <v>3318344</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="10">
-        <f>G16+G17+G18+G19+G20+G21+G22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="13">
-        <v>0</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="13">
-        <v>0</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="13">
-        <v>0</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="C19" s="14">
-        <f>B2*C2*B19</f>
-        <v>3318344</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="13">
-        <v>0</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="13">
-        <v>0</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="13">
-        <v>0</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5">
+        <f>127006*Agriculture!A2*Agriculture!B2/1000000</f>
+        <v>4318204</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5">
+        <f>730000*A2/1000000</f>
+        <v>2422391.12</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="5">
+        <f>(B9-B10)/4000</f>
+        <v>473.95321999999999</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="16"/>
     </row>
   </sheetData>
@@ -1098,104 +878,445 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12">
+        <v>259000</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12">
+        <v>571500</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12">
+        <v>14344</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12">
+        <v>571500</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>571500</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12">
+        <v>571500</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="11">
+        <v>7</v>
+      </c>
+      <c r="C8" s="12">
+        <v>259000</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="12">
+        <v>500000</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="10"/>
+      <c r="B1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="20">
+        <f>C2+C3+C4+C5+C6+C7+C8</f>
+        <v>3318344</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="11">
+        <f>G2+G3+G4+G5+G6+G7+G8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="14">
+        <f>General!A2*General!C6*B5</f>
+        <v>3318344</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>200000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="12">
-        <v>2318344</v>
-      </c>
-      <c r="C2" s="1">
-        <v>200000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>170</v>
-      </c>
-    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="5">
-        <f>127006*C2*D2/1000000</f>
-        <v>4318204</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>50</v>
+      <c r="A5" t="s">
+        <v>48</v>
       </c>
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="5">
-        <f>730000*B2/1000000</f>
-        <v>1692391.12</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>50</v>
+      <c r="A6" t="s">
+        <v>66</v>
       </c>
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="5">
-        <f>B5-B6</f>
-        <v>2625812.88</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>50</v>
+      <c r="A7" t="s">
+        <v>67</v>
       </c>
       <c r="E7" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D15" s="8"/>

</xml_diff>